<commit_message>
TASK 162419-NIMBIS Pull request-Assests,Contents
</commit_message>
<xml_diff>
--- a/src/NIMBIS.xlsx
+++ b/src/NIMBIS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SandhiyaM\Documents\GitHub\qa-automation-nimbus\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prave\IdeaProjects\qa-automation-nimbus\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B0A62A-E176-4BE4-9A29-CD80B754BFDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90BD1F09-1801-4D95-9C8F-28E8CAB3D9C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23016" windowHeight="11232" firstSheet="7" activeTab="10" xr2:uid="{A48C591E-A447-324F-80BA-5B973C426F33}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="6" xr2:uid="{A48C591E-A447-324F-80BA-5B973C426F33}"/>
   </bookViews>
   <sheets>
     <sheet name=" Client Test cases" sheetId="2" r:id="rId1"/>
@@ -1624,7 +1624,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2068,25 +2068,25 @@
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="28.453125" customWidth="1"/>
+    <col min="3" max="3" width="28.5" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="18.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="18.09765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.3984375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.09765625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="23" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="25.81640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="23.453125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="27.453125" customWidth="1"/>
-    <col min="33" max="34" width="31.6328125" customWidth="1"/>
-    <col min="43" max="43" width="33.90625" customWidth="1"/>
+    <col min="27" max="27" width="25.796875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="27.5" customWidth="1"/>
+    <col min="33" max="34" width="31.59765625" customWidth="1"/>
+    <col min="43" max="43" width="33.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>47</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:43">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2270,7 +2270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:43">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:43">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:43">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2429,7 +2429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:43">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2482,7 +2482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:43">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2535,7 +2535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:43">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2588,7 +2588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:43">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2641,7 +2641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:43">
+    <row r="10" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2694,7 +2694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:43">
+    <row r="11" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2747,7 +2747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:43">
+    <row r="12" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:43">
+    <row r="13" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2853,7 +2853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:43">
+    <row r="14" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2906,7 +2906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:43">
+    <row r="15" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2959,7 +2959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:43">
+    <row r="16" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -3012,7 +3012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:43">
+    <row r="17" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -3065,7 +3065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:43">
+    <row r="18" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -3118,7 +3118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:43">
+    <row r="19" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -3171,7 +3171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:43">
+    <row r="20" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -3224,7 +3224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:43">
+    <row r="21" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -3277,7 +3277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:43">
+    <row r="22" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -3330,7 +3330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:43">
+    <row r="23" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -3383,7 +3383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:43">
+    <row r="24" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -3436,7 +3436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:43">
+    <row r="25" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -3489,7 +3489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:43">
+    <row r="26" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -3542,7 +3542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:43">
+    <row r="27" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -3595,7 +3595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:43">
+    <row r="28" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -3648,7 +3648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:43">
+    <row r="29" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
@@ -3701,7 +3701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:43">
+    <row r="30" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
@@ -3754,7 +3754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:43">
+    <row r="31" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
@@ -3807,7 +3807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:43">
+    <row r="32" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -3860,7 +3860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:43">
+    <row r="33" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
@@ -3913,7 +3913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:43">
+    <row r="34" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
@@ -3966,7 +3966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:43">
+    <row r="35" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
@@ -4019,7 +4019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:43">
+    <row r="36" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
@@ -4072,7 +4072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:43">
+    <row r="37" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
@@ -4125,7 +4125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:43">
+    <row r="38" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
@@ -4178,7 +4178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:43">
+    <row r="39" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
@@ -4231,7 +4231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:43">
+    <row r="40" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
@@ -4284,7 +4284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:43">
+    <row r="41" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
@@ -4338,11 +4338,8 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH2:AH41" xr:uid="{7C05C23F-F7F1-D146-BB61-B78F3DCD95D3}">
-      <formula1>#REF!</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D41 L2:M41" xr:uid="{2DFC92E4-F910-FC46-AE0F-88E90FD645CD}">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH2:AH41 C2:D41 L2:M41" xr:uid="{7C05C23F-F7F1-D146-BB61-B78F3DCD95D3}">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -4359,14 +4356,14 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="25.54296875" customWidth="1"/>
+    <col min="2" max="2" width="25.5" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="5" max="5" width="29.90625" customWidth="1"/>
+    <col min="5" max="5" width="29.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>47</v>
       </c>
@@ -4383,7 +4380,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4397,7 +4394,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4411,7 +4408,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4434,13 +4431,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3FD076E-D013-450C-B736-C885ECA3A723}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>412</v>
       </c>
@@ -4454,7 +4451,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4465,7 +4462,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4476,7 +4473,7 @@
         <v>75000</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4487,7 +4484,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4511,368 +4508,368 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="152.453125" customWidth="1"/>
-    <col min="2" max="2" width="29.08984375" customWidth="1"/>
+    <col min="1" max="1" width="152.5" customWidth="1"/>
+    <col min="2" max="2" width="29.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>141</v>
       </c>
@@ -4890,29 +4887,29 @@
       <selection activeCell="B150" sqref="B150"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="64.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="28.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.8984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="28.19921875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="30.1796875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.6328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.54296875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="45.54296875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="23.08984375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.09765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30.19921875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.19921875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.59765625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="45.5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="23.09765625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="23.19921875" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="21" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="33.81640625" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="33.796875" bestFit="1" customWidth="1"/>
     <col min="64" max="65" width="44" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65">
+    <row r="1" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>47</v>
       </c>
@@ -5109,7 +5106,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="2" spans="1:65">
+    <row r="2" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5252,7 +5249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:65">
+    <row r="3" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5395,7 +5392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:65">
+    <row r="4" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5538,7 +5535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:65">
+    <row r="5" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5681,7 +5678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:65">
+    <row r="6" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -5824,7 +5821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:65">
+    <row r="7" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -5967,7 +5964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:65">
+    <row r="8" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -6110,7 +6107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:65">
+    <row r="9" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -6253,7 +6250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:65">
+    <row r="10" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -6396,7 +6393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:65">
+    <row r="11" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -6539,7 +6536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:65">
+    <row r="12" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -6682,7 +6679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:65">
+    <row r="13" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -6825,7 +6822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:65">
+    <row r="14" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -6968,7 +6965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:65">
+    <row r="15" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -7111,7 +7108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:65">
+    <row r="16" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -7254,7 +7251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:65">
+    <row r="17" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -7397,7 +7394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:65">
+    <row r="18" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -7540,7 +7537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:65">
+    <row r="19" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -7683,7 +7680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:65">
+    <row r="20" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -7826,7 +7823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:65">
+    <row r="21" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -7969,7 +7966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:65">
+    <row r="22" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -8112,7 +8109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:65">
+    <row r="23" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -8255,7 +8252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:65">
+    <row r="24" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -8398,7 +8395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:65" ht="14.25" customHeight="1">
+    <row r="25" spans="1:65" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -8541,7 +8538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:65">
+    <row r="26" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -8684,7 +8681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:65">
+    <row r="27" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -8827,7 +8824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:65">
+    <row r="28" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -8970,7 +8967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:65">
+    <row r="29" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -9113,7 +9110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:65">
+    <row r="30" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -9256,7 +9253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:65">
+    <row r="31" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -9399,7 +9396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:65">
+    <row r="32" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -9542,7 +9539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:65">
+    <row r="33" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -9685,7 +9682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:65">
+    <row r="34" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -9828,7 +9825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:65">
+    <row r="35" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -9971,7 +9968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:65">
+    <row r="36" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -10114,7 +10111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:65">
+    <row r="37" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -10257,7 +10254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:65">
+    <row r="38" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -10400,7 +10397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:65">
+    <row r="39" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -10543,7 +10540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:65">
+    <row r="40" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -10686,7 +10683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:65">
+    <row r="41" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -10829,7 +10826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:65">
+    <row r="42" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -10972,7 +10969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:65">
+    <row r="43" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -11115,7 +11112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:65">
+    <row r="44" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -11258,7 +11255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:65">
+    <row r="45" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -11401,7 +11398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:65">
+    <row r="46" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -11544,7 +11541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:65">
+    <row r="47" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -11687,7 +11684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:65">
+    <row r="48" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -11830,7 +11827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:65">
+    <row r="49" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -11973,7 +11970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:65">
+    <row r="50" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -12116,7 +12113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:65">
+    <row r="51" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -12259,7 +12256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:65">
+    <row r="52" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -12402,7 +12399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:65">
+    <row r="53" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -12545,7 +12542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:65">
+    <row r="54" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -12688,7 +12685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:65">
+    <row r="55" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -12843,7 +12840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:65">
+    <row r="56" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -12986,7 +12983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:65">
+    <row r="57" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -13129,7 +13126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:65">
+    <row r="58" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -13272,7 +13269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:65">
+    <row r="59" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -13415,7 +13412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:65">
+    <row r="60" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -13558,7 +13555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:65">
+    <row r="61" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -13701,7 +13698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:65">
+    <row r="62" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -13844,7 +13841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:65">
+    <row r="63" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -13987,7 +13984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:65">
+    <row r="64" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -14130,7 +14127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:65">
+    <row r="65" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -14273,7 +14270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:65">
+    <row r="66" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
@@ -14416,7 +14413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:65">
+    <row r="67" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
@@ -14559,7 +14556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:65">
+    <row r="68" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
@@ -14702,7 +14699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:65">
+    <row r="69" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
@@ -14845,7 +14842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:65">
+    <row r="70" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
@@ -14988,7 +14985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:65">
+    <row r="71" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
@@ -15131,7 +15128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:65">
+    <row r="72" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
@@ -15274,7 +15271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:65">
+    <row r="73" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
@@ -15417,7 +15414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:65">
+    <row r="74" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>73</v>
       </c>
@@ -15560,7 +15557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:65">
+    <row r="75" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>74</v>
       </c>
@@ -15703,7 +15700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:65">
+    <row r="76" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>75</v>
       </c>
@@ -15846,7 +15843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:65">
+    <row r="77" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>76</v>
       </c>
@@ -15989,7 +15986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:65">
+    <row r="78" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>77</v>
       </c>
@@ -16132,7 +16129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:65">
+    <row r="79" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>78</v>
       </c>
@@ -16275,7 +16272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:65">
+    <row r="80" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>79</v>
       </c>
@@ -16418,7 +16415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:65">
+    <row r="81" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>80</v>
       </c>
@@ -16561,7 +16558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:65">
+    <row r="82" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>81</v>
       </c>
@@ -16704,7 +16701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:65">
+    <row r="83" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>82</v>
       </c>
@@ -16847,7 +16844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:65">
+    <row r="84" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>83</v>
       </c>
@@ -16990,7 +16987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:65">
+    <row r="85" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>84</v>
       </c>
@@ -17133,7 +17130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:65">
+    <row r="86" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>85</v>
       </c>
@@ -17276,7 +17273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:65">
+    <row r="87" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>86</v>
       </c>
@@ -17419,7 +17416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:65">
+    <row r="88" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>87</v>
       </c>
@@ -17562,7 +17559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:65">
+    <row r="89" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>88</v>
       </c>
@@ -17705,7 +17702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:65">
+    <row r="90" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>89</v>
       </c>
@@ -17848,7 +17845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:65">
+    <row r="91" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>90</v>
       </c>
@@ -17991,7 +17988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:65">
+    <row r="92" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>91</v>
       </c>
@@ -18134,7 +18131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:65">
+    <row r="93" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>92</v>
       </c>
@@ -18277,7 +18274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:65">
+    <row r="94" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>93</v>
       </c>
@@ -18420,7 +18417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:65">
+    <row r="95" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>94</v>
       </c>
@@ -18563,7 +18560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:65">
+    <row r="96" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>95</v>
       </c>
@@ -18706,7 +18703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:65">
+    <row r="97" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>96</v>
       </c>
@@ -18849,7 +18846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:65">
+    <row r="98" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>97</v>
       </c>
@@ -18992,7 +18989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:65">
+    <row r="99" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>98</v>
       </c>
@@ -19135,7 +19132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:65">
+    <row r="100" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>99</v>
       </c>
@@ -19278,7 +19275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:65">
+    <row r="101" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>100</v>
       </c>
@@ -19421,7 +19418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:65">
+    <row r="102" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>101</v>
       </c>
@@ -19564,7 +19561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:65">
+    <row r="103" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>102</v>
       </c>
@@ -19707,7 +19704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:65">
+    <row r="104" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>103</v>
       </c>
@@ -19850,7 +19847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:65">
+    <row r="105" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>104</v>
       </c>
@@ -19993,7 +19990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:65">
+    <row r="106" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>105</v>
       </c>
@@ -20136,7 +20133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:65">
+    <row r="107" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>106</v>
       </c>
@@ -20279,7 +20276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:65">
+    <row r="108" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>107</v>
       </c>
@@ -20422,7 +20419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:65">
+    <row r="109" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>108</v>
       </c>
@@ -20565,7 +20562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:65">
+    <row r="110" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>109</v>
       </c>
@@ -20708,7 +20705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:65">
+    <row r="111" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>110</v>
       </c>
@@ -20851,7 +20848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:65">
+    <row r="112" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>111</v>
       </c>
@@ -20994,7 +20991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:65">
+    <row r="113" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>112</v>
       </c>
@@ -21137,7 +21134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:65">
+    <row r="114" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>113</v>
       </c>
@@ -21280,7 +21277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:65">
+    <row r="115" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>114</v>
       </c>
@@ -21423,7 +21420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:65">
+    <row r="116" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>115</v>
       </c>
@@ -21566,7 +21563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:65">
+    <row r="117" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>116</v>
       </c>
@@ -21709,7 +21706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:65">
+    <row r="118" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>117</v>
       </c>
@@ -21852,7 +21849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:65">
+    <row r="119" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>118</v>
       </c>
@@ -21995,7 +21992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:65">
+    <row r="120" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>119</v>
       </c>
@@ -22138,7 +22135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:65">
+    <row r="121" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>120</v>
       </c>
@@ -22281,7 +22278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:65">
+    <row r="122" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>121</v>
       </c>
@@ -22424,7 +22421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:65">
+    <row r="123" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>122</v>
       </c>
@@ -22567,7 +22564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:65">
+    <row r="124" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>123</v>
       </c>
@@ -22710,7 +22707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:65">
+    <row r="125" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>124</v>
       </c>
@@ -22853,7 +22850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:65">
+    <row r="126" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>125</v>
       </c>
@@ -22996,7 +22993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:65">
+    <row r="127" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>126</v>
       </c>
@@ -23139,7 +23136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:65">
+    <row r="128" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>127</v>
       </c>
@@ -23282,7 +23279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:65">
+    <row r="129" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>128</v>
       </c>
@@ -23425,7 +23422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:65">
+    <row r="130" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>129</v>
       </c>
@@ -23568,7 +23565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:65">
+    <row r="131" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>130</v>
       </c>
@@ -23711,7 +23708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:65">
+    <row r="132" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>131</v>
       </c>
@@ -23854,7 +23851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:65">
+    <row r="133" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>132</v>
       </c>
@@ -23997,7 +23994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:65">
+    <row r="134" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>133</v>
       </c>
@@ -24140,7 +24137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:65">
+    <row r="135" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>134</v>
       </c>
@@ -24283,7 +24280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:65">
+    <row r="136" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>135</v>
       </c>
@@ -24426,7 +24423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:65">
+    <row r="137" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>136</v>
       </c>
@@ -24569,7 +24566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:65">
+    <row r="138" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>137</v>
       </c>
@@ -24712,7 +24709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:65">
+    <row r="139" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>138</v>
       </c>
@@ -24855,7 +24852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:65">
+    <row r="140" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>139</v>
       </c>
@@ -24998,7 +24995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:65">
+    <row r="141" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>140</v>
       </c>
@@ -25141,7 +25138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:65">
+    <row r="142" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>141</v>
       </c>
@@ -25284,7 +25281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:65">
+    <row r="143" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>142</v>
       </c>
@@ -25427,7 +25424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:65">
+    <row r="144" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>143</v>
       </c>
@@ -25570,7 +25567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:65">
+    <row r="145" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>144</v>
       </c>
@@ -25713,7 +25710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:65">
+    <row r="146" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>145</v>
       </c>
@@ -25856,7 +25853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:65">
+    <row r="147" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>146</v>
       </c>
@@ -25999,7 +25996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:65">
+    <row r="148" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>147</v>
       </c>
@@ -26145,7 +26142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:65">
+    <row r="149" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>148</v>
       </c>
@@ -26291,7 +26288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:65">
+    <row r="150" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>149</v>
       </c>
@@ -26437,7 +26434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:65">
+    <row r="151" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>150</v>
       </c>
@@ -26583,7 +26580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:65">
+    <row r="152" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>151</v>
       </c>
@@ -26729,7 +26726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:65">
+    <row r="153" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>152</v>
       </c>
@@ -26875,7 +26872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:65">
+    <row r="154" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>153</v>
       </c>
@@ -27021,7 +27018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:65">
+    <row r="155" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>154</v>
       </c>
@@ -27167,7 +27164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:65">
+    <row r="156" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>155</v>
       </c>
@@ -27313,7 +27310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:65">
+    <row r="157" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>156</v>
       </c>
@@ -27456,7 +27453,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="158" spans="1:65">
+    <row r="158" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>157</v>
       </c>
@@ -27599,7 +27596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:65">
+    <row r="159" spans="1:65" x14ac:dyDescent="0.3">
       <c r="AC159">
         <v>1</v>
       </c>
@@ -27634,16 +27631,16 @@
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="28.36328125" customWidth="1"/>
-    <col min="3" max="3" width="12.26953125" customWidth="1"/>
+    <col min="2" max="2" width="28.3984375" customWidth="1"/>
+    <col min="3" max="3" width="12.296875" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="23.7265625" customWidth="1"/>
-    <col min="6" max="6" width="21.453125" customWidth="1"/>
+    <col min="5" max="5" width="23.69921875" customWidth="1"/>
+    <col min="6" max="6" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>343</v>
       </c>
@@ -27663,7 +27660,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -27680,7 +27677,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -27697,7 +27694,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -27714,7 +27711,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -27731,7 +27728,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -27748,7 +27745,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -27765,7 +27762,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -27782,7 +27779,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -27799,7 +27796,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -27829,13 +27826,13 @@
       <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>223</v>
       </c>
@@ -27843,7 +27840,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>342</v>
       </c>
@@ -27868,13 +27865,13 @@
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.08984375" customWidth="1"/>
-    <col min="9" max="9" width="22.36328125" customWidth="1"/>
+    <col min="2" max="2" width="19.09765625" customWidth="1"/>
+    <col min="9" max="9" width="22.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:70">
+    <row r="1" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>47</v>
       </c>
@@ -28050,7 +28047,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="2" spans="1:70">
+    <row r="2" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -28187,7 +28184,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="3" spans="1:70">
+    <row r="3" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -28324,7 +28321,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="4" spans="1:70">
+    <row r="4" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -28461,7 +28458,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="5" spans="1:70">
+    <row r="5" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -28598,7 +28595,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="6" spans="1:70">
+    <row r="6" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -28735,7 +28732,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="7" spans="1:70">
+    <row r="7" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -28872,7 +28869,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="8" spans="1:70">
+    <row r="8" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -29009,7 +29006,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:70">
+    <row r="9" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -29146,7 +29143,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="10" spans="1:70">
+    <row r="10" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -29283,7 +29280,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="11" spans="1:70">
+    <row r="11" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -29420,7 +29417,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="12" spans="1:70">
+    <row r="12" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -29557,7 +29554,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="13" spans="1:70">
+    <row r="13" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -29694,7 +29691,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="14" spans="1:70">
+    <row r="14" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -29831,7 +29828,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="15" spans="1:70">
+    <row r="15" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -29968,7 +29965,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="16" spans="1:70">
+    <row r="16" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -30105,7 +30102,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="17" spans="1:70">
+    <row r="17" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -30242,7 +30239,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="18" spans="1:70">
+    <row r="18" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -30379,7 +30376,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="19" spans="1:70">
+    <row r="19" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -30516,7 +30513,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="20" spans="1:70">
+    <row r="20" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -30653,7 +30650,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="21" spans="1:70">
+    <row r="21" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -30790,7 +30787,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="22" spans="1:70">
+    <row r="22" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -30927,7 +30924,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="23" spans="1:70">
+    <row r="23" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -31064,7 +31061,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="24" spans="1:70">
+    <row r="24" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -31201,7 +31198,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="25" spans="1:70">
+    <row r="25" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -31338,7 +31335,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="26" spans="1:70">
+    <row r="26" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -31475,7 +31472,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="27" spans="1:70">
+    <row r="27" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -31612,7 +31609,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="28" spans="1:70">
+    <row r="28" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -31749,7 +31746,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="29" spans="1:70">
+    <row r="29" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -31886,7 +31883,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="30" spans="1:70">
+    <row r="30" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -32023,7 +32020,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="31" spans="1:70">
+    <row r="31" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -32160,7 +32157,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="32" spans="1:70">
+    <row r="32" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -32297,7 +32294,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="33" spans="1:70">
+    <row r="33" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -32434,7 +32431,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="34" spans="1:70">
+    <row r="34" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -32571,7 +32568,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="35" spans="1:70">
+    <row r="35" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -32708,7 +32705,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="36" spans="1:70">
+    <row r="36" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -32845,7 +32842,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="37" spans="1:70">
+    <row r="37" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -32982,7 +32979,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="38" spans="1:70">
+    <row r="38" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -33119,7 +33116,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="39" spans="1:70">
+    <row r="39" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -33256,7 +33253,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="40" spans="1:70">
+    <row r="40" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -33393,7 +33390,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="41" spans="1:70">
+    <row r="41" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -33530,7 +33527,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="42" spans="1:70">
+    <row r="42" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -33667,7 +33664,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="43" spans="1:70">
+    <row r="43" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -33804,7 +33801,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="44" spans="1:70">
+    <row r="44" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -33941,7 +33938,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="45" spans="1:70">
+    <row r="45" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -34078,7 +34075,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="46" spans="1:70">
+    <row r="46" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -34215,7 +34212,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="47" spans="1:70">
+    <row r="47" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -34352,7 +34349,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="48" spans="1:70">
+    <row r="48" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -34489,7 +34486,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="49" spans="1:70">
+    <row r="49" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -34626,7 +34623,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="50" spans="1:70">
+    <row r="50" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -34763,7 +34760,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="51" spans="1:70">
+    <row r="51" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -34900,7 +34897,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="52" spans="1:70">
+    <row r="52" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -35037,7 +35034,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="53" spans="1:70">
+    <row r="53" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -35174,7 +35171,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="54" spans="1:70">
+    <row r="54" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -35311,7 +35308,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="55" spans="1:70">
+    <row r="55" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -35448,7 +35445,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="56" spans="1:70">
+    <row r="56" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -35585,7 +35582,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="57" spans="1:70">
+    <row r="57" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -35722,7 +35719,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="58" spans="1:70">
+    <row r="58" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -35859,7 +35856,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="59" spans="1:70">
+    <row r="59" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -35996,7 +35993,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="60" spans="1:70">
+    <row r="60" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -36133,7 +36130,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="61" spans="1:70">
+    <row r="61" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -36270,7 +36267,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="62" spans="1:70">
+    <row r="62" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -36407,7 +36404,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="63" spans="1:70">
+    <row r="63" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -36544,7 +36541,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="64" spans="1:70">
+    <row r="64" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -36681,7 +36678,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="65" spans="1:70">
+    <row r="65" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -36818,7 +36815,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="66" spans="1:70">
+    <row r="66" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
@@ -36955,7 +36952,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="67" spans="1:70">
+    <row r="67" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
@@ -37092,7 +37089,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="68" spans="1:70">
+    <row r="68" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
@@ -37229,7 +37226,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="69" spans="1:70">
+    <row r="69" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
@@ -37366,7 +37363,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="70" spans="1:70">
+    <row r="70" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
@@ -37503,7 +37500,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="71" spans="1:70">
+    <row r="71" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
@@ -37640,7 +37637,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="72" spans="1:70">
+    <row r="72" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
@@ -37777,7 +37774,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="73" spans="1:70">
+    <row r="73" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
@@ -37914,7 +37911,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="74" spans="1:70">
+    <row r="74" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>73</v>
       </c>
@@ -38051,7 +38048,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="75" spans="1:70">
+    <row r="75" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>74</v>
       </c>
@@ -38188,7 +38185,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="76" spans="1:70">
+    <row r="76" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>75</v>
       </c>
@@ -38325,7 +38322,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="77" spans="1:70">
+    <row r="77" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>76</v>
       </c>
@@ -38462,7 +38459,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="78" spans="1:70">
+    <row r="78" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>77</v>
       </c>
@@ -38599,7 +38596,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="79" spans="1:70">
+    <row r="79" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>78</v>
       </c>
@@ -38736,7 +38733,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="80" spans="1:70">
+    <row r="80" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>79</v>
       </c>
@@ -38873,7 +38870,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="81" spans="1:70">
+    <row r="81" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>80</v>
       </c>
@@ -39010,7 +39007,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="82" spans="1:70">
+    <row r="82" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>81</v>
       </c>
@@ -39147,7 +39144,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="83" spans="1:70">
+    <row r="83" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>82</v>
       </c>
@@ -39284,7 +39281,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="84" spans="1:70">
+    <row r="84" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>83</v>
       </c>
@@ -39421,7 +39418,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="85" spans="1:70">
+    <row r="85" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>84</v>
       </c>
@@ -39558,7 +39555,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="86" spans="1:70">
+    <row r="86" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>85</v>
       </c>
@@ -39695,7 +39692,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="87" spans="1:70">
+    <row r="87" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>86</v>
       </c>
@@ -39832,7 +39829,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="88" spans="1:70">
+    <row r="88" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>87</v>
       </c>
@@ -39969,7 +39966,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="89" spans="1:70">
+    <row r="89" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>88</v>
       </c>
@@ -40106,7 +40103,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="90" spans="1:70">
+    <row r="90" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>89</v>
       </c>
@@ -40243,7 +40240,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="91" spans="1:70">
+    <row r="91" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>90</v>
       </c>
@@ -40380,7 +40377,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="92" spans="1:70">
+    <row r="92" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>91</v>
       </c>
@@ -40517,7 +40514,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="93" spans="1:70">
+    <row r="93" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>92</v>
       </c>
@@ -40654,7 +40651,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="94" spans="1:70">
+    <row r="94" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>94</v>
       </c>
@@ -40791,7 +40788,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="95" spans="1:70">
+    <row r="95" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>96</v>
       </c>
@@ -40928,7 +40925,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="96" spans="1:70">
+    <row r="96" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>97</v>
       </c>
@@ -41068,7 +41065,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="97" spans="1:70">
+    <row r="97" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>98</v>
       </c>
@@ -41205,7 +41202,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="98" spans="1:70">
+    <row r="98" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>99</v>
       </c>
@@ -41342,7 +41339,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="99" spans="1:70">
+    <row r="99" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>100</v>
       </c>
@@ -41479,7 +41476,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="100" spans="1:70">
+    <row r="100" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>101</v>
       </c>
@@ -41616,7 +41613,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="101" spans="1:70">
+    <row r="101" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>102</v>
       </c>
@@ -41753,7 +41750,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="102" spans="1:70">
+    <row r="102" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>103</v>
       </c>
@@ -41890,7 +41887,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="103" spans="1:70">
+    <row r="103" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>104</v>
       </c>
@@ -42027,7 +42024,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="104" spans="1:70">
+    <row r="104" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>105</v>
       </c>
@@ -42164,7 +42161,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="105" spans="1:70">
+    <row r="105" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>106</v>
       </c>
@@ -42301,7 +42298,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="106" spans="1:70">
+    <row r="106" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>107</v>
       </c>
@@ -42438,7 +42435,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="107" spans="1:70">
+    <row r="107" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>109</v>
       </c>
@@ -42575,7 +42572,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="108" spans="1:70">
+    <row r="108" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>110</v>
       </c>
@@ -42712,7 +42709,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="109" spans="1:70">
+    <row r="109" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>111</v>
       </c>
@@ -42849,7 +42846,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="110" spans="1:70">
+    <row r="110" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>112</v>
       </c>
@@ -42986,7 +42983,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="111" spans="1:70">
+    <row r="111" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>113</v>
       </c>
@@ -43123,7 +43120,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="112" spans="1:70">
+    <row r="112" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>114</v>
       </c>
@@ -43260,7 +43257,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="113" spans="1:70">
+    <row r="113" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>115</v>
       </c>
@@ -43397,7 +43394,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="114" spans="1:70">
+    <row r="114" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>116</v>
       </c>
@@ -43534,7 +43531,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="115" spans="1:70">
+    <row r="115" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>117</v>
       </c>
@@ -43671,7 +43668,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="116" spans="1:70">
+    <row r="116" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>118</v>
       </c>
@@ -43808,7 +43805,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="117" spans="1:70">
+    <row r="117" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>119</v>
       </c>
@@ -43945,7 +43942,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="118" spans="1:70">
+    <row r="118" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>120</v>
       </c>
@@ -44082,7 +44079,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="119" spans="1:70">
+    <row r="119" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>121</v>
       </c>
@@ -44219,7 +44216,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="120" spans="1:70">
+    <row r="120" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>122</v>
       </c>
@@ -44356,7 +44353,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="121" spans="1:70">
+    <row r="121" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>123</v>
       </c>
@@ -44493,7 +44490,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="122" spans="1:70">
+    <row r="122" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>124</v>
       </c>
@@ -44630,7 +44627,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="123" spans="1:70">
+    <row r="123" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>125</v>
       </c>
@@ -44767,7 +44764,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="124" spans="1:70">
+    <row r="124" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>126</v>
       </c>
@@ -44904,7 +44901,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="125" spans="1:70">
+    <row r="125" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>127</v>
       </c>
@@ -45041,7 +45038,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="126" spans="1:70">
+    <row r="126" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>128</v>
       </c>
@@ -45178,7 +45175,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="127" spans="1:70">
+    <row r="127" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>129</v>
       </c>
@@ -45315,7 +45312,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="128" spans="1:70">
+    <row r="128" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>130</v>
       </c>
@@ -45452,7 +45449,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="129" spans="1:70">
+    <row r="129" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>131</v>
       </c>
@@ -45589,7 +45586,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="130" spans="1:70">
+    <row r="130" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>132</v>
       </c>
@@ -45726,7 +45723,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="131" spans="1:70">
+    <row r="131" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>133</v>
       </c>
@@ -45863,7 +45860,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="132" spans="1:70">
+    <row r="132" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>134</v>
       </c>
@@ -46000,7 +45997,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="133" spans="1:70">
+    <row r="133" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>135</v>
       </c>
@@ -46137,7 +46134,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="134" spans="1:70">
+    <row r="134" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>136</v>
       </c>
@@ -46274,7 +46271,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="135" spans="1:70">
+    <row r="135" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>137</v>
       </c>
@@ -46411,7 +46408,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="136" spans="1:70">
+    <row r="136" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>138</v>
       </c>
@@ -46548,7 +46545,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="137" spans="1:70">
+    <row r="137" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>139</v>
       </c>
@@ -46685,7 +46682,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="138" spans="1:70">
+    <row r="138" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>140</v>
       </c>
@@ -46822,7 +46819,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="139" spans="1:70">
+    <row r="139" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>141</v>
       </c>
@@ -46959,7 +46956,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="140" spans="1:70">
+    <row r="140" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>142</v>
       </c>
@@ -47096,7 +47093,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="141" spans="1:70">
+    <row r="141" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>143</v>
       </c>
@@ -47233,7 +47230,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="142" spans="1:70">
+    <row r="142" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>144</v>
       </c>
@@ -47370,7 +47367,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="143" spans="1:70">
+    <row r="143" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>145</v>
       </c>
@@ -47507,7 +47504,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="144" spans="1:70">
+    <row r="144" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>146</v>
       </c>
@@ -47644,7 +47641,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="145" spans="1:70">
+    <row r="145" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>147</v>
       </c>
@@ -47781,7 +47778,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="146" spans="1:70">
+    <row r="146" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>148</v>
       </c>
@@ -47918,7 +47915,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="147" spans="1:70">
+    <row r="147" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>149</v>
       </c>
@@ -48055,7 +48052,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="148" spans="1:70">
+    <row r="148" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>150</v>
       </c>
@@ -48192,7 +48189,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="149" spans="1:70">
+    <row r="149" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>151</v>
       </c>
@@ -48329,7 +48326,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="150" spans="1:70">
+    <row r="150" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>152</v>
       </c>
@@ -48466,7 +48463,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="151" spans="1:70">
+    <row r="151" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>153</v>
       </c>
@@ -48603,7 +48600,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="152" spans="1:70">
+    <row r="152" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>154</v>
       </c>
@@ -48740,7 +48737,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="153" spans="1:70">
+    <row r="153" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>155</v>
       </c>
@@ -48877,7 +48874,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="154" spans="1:70">
+    <row r="154" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>156</v>
       </c>
@@ -49014,7 +49011,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="155" spans="1:70">
+    <row r="155" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>157</v>
       </c>
@@ -49151,7 +49148,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="156" spans="1:70">
+    <row r="156" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>158</v>
       </c>
@@ -49288,7 +49285,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="157" spans="1:70">
+    <row r="157" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>159</v>
       </c>
@@ -49425,7 +49422,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="158" spans="1:70">
+    <row r="158" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>160</v>
       </c>
@@ -49562,7 +49559,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="159" spans="1:70">
+    <row r="159" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>161</v>
       </c>
@@ -49699,7 +49696,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="160" spans="1:70">
+    <row r="160" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>162</v>
       </c>
@@ -49836,7 +49833,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="161" spans="1:70">
+    <row r="161" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>163</v>
       </c>
@@ -49988,9 +49985,9 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:28" ht="45">
+    <row r="1" spans="1:28" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>343</v>
       </c>
@@ -50076,7 +50073,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -50132,7 +50129,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -50188,7 +50185,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:28">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -50244,7 +50241,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:28">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -50300,7 +50297,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:28">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -50356,7 +50353,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:28">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -50412,7 +50409,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:28">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -50468,7 +50465,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:28">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -50524,7 +50521,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:28">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -50580,7 +50577,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:28">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -50636,7 +50633,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:28">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -50692,7 +50689,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:28">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -50748,7 +50745,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:28">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -50804,7 +50801,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:28">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -50860,7 +50857,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:28">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -50916,7 +50913,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:28">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -50972,7 +50969,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:28">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -51037,13 +51034,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59041EA9-8709-4AB5-8382-8D75AFDF5A6B}">
   <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>412</v>
       </c>
@@ -51093,7 +51090,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -51128,7 +51125,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -51163,7 +51160,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -51198,7 +51195,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -51233,7 +51230,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -51268,7 +51265,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -51303,7 +51300,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -51338,7 +51335,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -51373,7 +51370,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -51408,7 +51405,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -51443,7 +51440,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -51478,7 +51475,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -51513,7 +51510,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -51548,7 +51545,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -51583,7 +51580,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -51618,7 +51615,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -51653,7 +51650,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -51688,7 +51685,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -51723,7 +51720,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -51758,7 +51755,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -51793,7 +51790,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -51828,7 +51825,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -51863,7 +51860,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -51898,7 +51895,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -51933,7 +51930,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -51968,7 +51965,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -52003,7 +52000,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -52051,9 +52048,9 @@
       <selection activeCell="V2" sqref="V2:V20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:30" ht="60">
+    <row r="1" spans="1:30" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>343</v>
       </c>
@@ -52145,7 +52142,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -52210,7 +52207,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -52275,7 +52272,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -52340,7 +52337,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -52405,7 +52402,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:30">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -52470,7 +52467,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:30">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -52535,7 +52532,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:30">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>8</v>
       </c>
@@ -52600,7 +52597,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:30" ht="60">
+    <row r="9" spans="1:30" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>9</v>
       </c>
@@ -52665,7 +52662,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:30">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>10</v>
       </c>
@@ -52730,7 +52727,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:30">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>11</v>
       </c>
@@ -52795,7 +52792,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:30">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>12</v>
       </c>
@@ -52860,7 +52857,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:30">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>13</v>
       </c>
@@ -52925,7 +52922,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:30">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>14</v>
       </c>
@@ -52990,7 +52987,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:30">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>15</v>
       </c>
@@ -53055,7 +53052,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:30">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>16</v>
       </c>
@@ -53120,7 +53117,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:30">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>17</v>
       </c>
@@ -53185,7 +53182,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:30">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>18</v>
       </c>
@@ -53250,7 +53247,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:30">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>19</v>
       </c>
@@ -53315,7 +53312,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:30">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>20</v>
       </c>
@@ -53393,9 +53390,9 @@
       <selection activeCell="B17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:18" ht="240">
+    <row r="1" spans="1:18" ht="249.6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>412</v>
       </c>
@@ -53451,7 +53448,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -53498,7 +53495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -53545,7 +53542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -53592,7 +53589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -53639,7 +53636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -53686,7 +53683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -53733,7 +53730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -53780,7 +53777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -53827,7 +53824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -53874,7 +53871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -53921,7 +53918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -53968,7 +53965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -54015,7 +54012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -54062,7 +54059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -54109,7 +54106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -54156,7 +54153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>19</v>
       </c>
@@ -54203,7 +54200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>20</v>
       </c>
@@ -54250,7 +54247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>21</v>
       </c>
@@ -54297,7 +54294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>22</v>
       </c>
@@ -54350,6 +54347,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="16e03651-acd4-40f0-82ea-ba55e12251a9" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="39c968c6-d81e-4a40-af5e-103bfa8ea621">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100974990A4B7481540AD2827693D2B4677" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="29dc9a2c723eb601f8a43bd90399fbaa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="39c968c6-d81e-4a40-af5e-103bfa8ea621" xmlns:ns3="16e03651-acd4-40f0-82ea-ba55e12251a9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9dea1e42ffc2c62d22e8c39d3144f8a7" ns2:_="" ns3:_="">
     <xsd:import namespace="39c968c6-d81e-4a40-af5e-103bfa8ea621"/>
@@ -54598,27 +54615,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DE6B354-43A9-4490-9EF5-3F7471DCEA9A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="16e03651-acd4-40f0-82ea-ba55e12251a9"/>
+    <ds:schemaRef ds:uri="39c968c6-d81e-4a40-af5e-103bfa8ea621"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="16e03651-acd4-40f0-82ea-ba55e12251a9" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="39c968c6-d81e-4a40-af5e-103bfa8ea621">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{488A6D9C-A748-45FA-846F-A9AD5EC1A9F6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF06F155-6F1A-4F06-A273-A2279113E9CD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -54635,23 +54651,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{488A6D9C-A748-45FA-846F-A9AD5EC1A9F6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DE6B354-43A9-4490-9EF5-3F7471DCEA9A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="16e03651-acd4-40f0-82ea-ba55e12251a9"/>
-    <ds:schemaRef ds:uri="39c968c6-d81e-4a40-af5e-103bfa8ea621"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>